<commit_message>
feat(ui): improve dashboard UX with smoother animations and tighter layout
- Add smooth slide animations for sidebar section collapse/expand
- Update CPF defaults from $3-5 to $0.50-1.00
- Change acquisition breakdown to horizontal month cards (no dropdown)
- Reduce padding across dashboard modules for tighter layout
- Make viz-panel background transparent to show darker body gradient
- Standardize title sizes between chart header and historical context
- Fix Pydantic schema field names (remove underscore prefix)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/public/Care Bears Audience Growth KPis .xlsx
+++ b/public/Care Bears Audience Growth KPis .xlsx
@@ -10,6 +10,7 @@
     <sheet state="visible" name="Projected Follower Growth" sheetId="5" r:id="rId8"/>
     <sheet state="visible" name="ChatGPT Figures" sheetId="6" r:id="rId9"/>
     <sheet state="visible" name="Competitor Benchmarks" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="Care Bears Data" sheetId="8" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="235">
   <si>
     <t>Channel</t>
   </si>
@@ -710,6 +711,24 @@
   <si>
     <t>22.7K</t>
   </si>
+  <si>
+    <t>Followers</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t># of posts</t>
+  </si>
+  <si>
+    <t>Engagement %</t>
+  </si>
+  <si>
+    <t>YouTube (Likes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YouTube </t>
+  </si>
 </sst>
 </file>
 
@@ -725,7 +744,7 @@
     <numFmt numFmtId="170" formatCode="mmmm yyyy"/>
     <numFmt numFmtId="171" formatCode="#.##K"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -802,8 +821,15 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -822,6 +848,18 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor rgb="FFF4CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE5CD"/>
+        <bgColor rgb="FFFCE5CD"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -829,7 +867,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="83">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1036,6 +1074,25 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="3" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="6" numFmtId="10" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="5" fontId="6" numFmtId="3" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="10" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1186,11 +1243,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="820846556"/>
-        <c:axId val="1027927022"/>
+        <c:axId val="2038947885"/>
+        <c:axId val="1414490006"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="820846556"/>
+        <c:axId val="2038947885"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1242,10 +1299,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1027927022"/>
+        <c:crossAx val="1414490006"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1027927022"/>
+        <c:axId val="1414490006"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1320,7 +1377,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="820846556"/>
+        <c:crossAx val="2038947885"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1422,11 +1479,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1577772788"/>
-        <c:axId val="1486397660"/>
+        <c:axId val="1111988849"/>
+        <c:axId val="542623716"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1577772788"/>
+        <c:axId val="1111988849"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1478,10 +1535,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1486397660"/>
+        <c:crossAx val="542623716"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1486397660"/>
+        <c:axId val="542623716"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1556,7 +1613,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1577772788"/>
+        <c:crossAx val="1111988849"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1666,6 +1723,10 @@
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -42208,4 +42269,993 @@
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="C2" sqref="C2" pane="topRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="15.75"/>
+  </cols>
+  <sheetData>
+    <row r="2">
+      <c r="A2" s="74" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="51">
+        <v>45627.0</v>
+      </c>
+      <c r="C2" s="51">
+        <v>45658.0</v>
+      </c>
+      <c r="D2" s="51">
+        <v>45689.0</v>
+      </c>
+      <c r="E2" s="51">
+        <v>45717.0</v>
+      </c>
+      <c r="F2" s="51">
+        <v>45748.0</v>
+      </c>
+      <c r="G2" s="51">
+        <v>45778.0</v>
+      </c>
+      <c r="H2" s="51">
+        <v>45809.0</v>
+      </c>
+      <c r="I2" s="51">
+        <v>45839.0</v>
+      </c>
+      <c r="J2" s="51">
+        <v>45870.0</v>
+      </c>
+      <c r="K2" s="51">
+        <v>45901.0</v>
+      </c>
+      <c r="L2" s="51">
+        <v>45931.0</v>
+      </c>
+      <c r="M2" s="51">
+        <v>45962.0</v>
+      </c>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="28">
+        <v>324000.0</v>
+      </c>
+      <c r="C3" s="28">
+        <v>330000.0</v>
+      </c>
+      <c r="D3" s="28">
+        <v>337000.0</v>
+      </c>
+      <c r="E3" s="28">
+        <v>343000.0</v>
+      </c>
+      <c r="F3" s="28">
+        <v>351000.0</v>
+      </c>
+      <c r="G3" s="28">
+        <v>357000.0</v>
+      </c>
+      <c r="H3" s="28">
+        <v>362000.0</v>
+      </c>
+      <c r="I3" s="28">
+        <v>367000.0</v>
+      </c>
+      <c r="J3" s="28">
+        <v>371000.0</v>
+      </c>
+      <c r="K3" s="28">
+        <v>373000.0</v>
+      </c>
+      <c r="L3" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="M3" s="28">
+        <v>381000.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="28">
+        <v>467000.0</v>
+      </c>
+      <c r="C4" s="28">
+        <v>471000.0</v>
+      </c>
+      <c r="D4" s="28">
+        <v>487000.0</v>
+      </c>
+      <c r="E4" s="28">
+        <v>493000.0</v>
+      </c>
+      <c r="F4" s="28">
+        <v>502000.0</v>
+      </c>
+      <c r="G4" s="28">
+        <v>505000.0</v>
+      </c>
+      <c r="H4" s="28">
+        <v>517000.0</v>
+      </c>
+      <c r="I4" s="28">
+        <v>536000.0</v>
+      </c>
+      <c r="J4" s="28">
+        <v>547000.0</v>
+      </c>
+      <c r="K4" s="28">
+        <v>551000.0</v>
+      </c>
+      <c r="L4" s="28">
+        <v>567101.0</v>
+      </c>
+      <c r="M4" s="28">
+        <v>573461.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="76">
+        <v>331168.0</v>
+      </c>
+      <c r="D5" s="76">
+        <v>331339.0</v>
+      </c>
+      <c r="E5" s="76">
+        <v>343900.0</v>
+      </c>
+      <c r="F5" s="76">
+        <v>337492.0</v>
+      </c>
+      <c r="G5" s="76">
+        <v>343394.0</v>
+      </c>
+      <c r="H5" s="76">
+        <v>345242.0</v>
+      </c>
+      <c r="I5" s="28">
+        <v>350290.0</v>
+      </c>
+      <c r="J5" s="28">
+        <v>359000.0</v>
+      </c>
+      <c r="K5" s="28">
+        <v>368000.0</v>
+      </c>
+      <c r="L5" s="28">
+        <v>378746.0</v>
+      </c>
+      <c r="M5" s="28">
+        <v>385208.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="76">
+        <v>531048.0</v>
+      </c>
+      <c r="D6" s="76">
+        <v>533307.0</v>
+      </c>
+      <c r="E6" s="76">
+        <v>535471.0</v>
+      </c>
+      <c r="F6" s="76">
+        <v>538295.0</v>
+      </c>
+      <c r="G6" s="76">
+        <v>543062.0</v>
+      </c>
+      <c r="H6" s="76">
+        <v>545309.0</v>
+      </c>
+      <c r="I6" s="28">
+        <v>552000.0</v>
+      </c>
+      <c r="J6" s="28">
+        <v>559000.0</v>
+      </c>
+      <c r="K6" s="28">
+        <v>568000.0</v>
+      </c>
+      <c r="L6" s="28">
+        <v>548059.0</v>
+      </c>
+      <c r="M6" s="28">
+        <v>592357.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="74" t="s">
+        <v>231</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="28">
+        <v>16.0</v>
+      </c>
+      <c r="E9" s="28">
+        <v>14.0</v>
+      </c>
+      <c r="F9" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="G9" s="28">
+        <v>3.0</v>
+      </c>
+      <c r="H9" s="28">
+        <v>8.0</v>
+      </c>
+      <c r="I9" s="28">
+        <v>4.0</v>
+      </c>
+      <c r="J9" s="28">
+        <v>4.0</v>
+      </c>
+      <c r="K9" s="28">
+        <v>3.0</v>
+      </c>
+      <c r="L9" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="M9" s="28">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="28">
+        <v>25.0</v>
+      </c>
+      <c r="D10" s="28">
+        <v>34.0</v>
+      </c>
+      <c r="E10" s="28">
+        <v>30.0</v>
+      </c>
+      <c r="F10" s="28">
+        <v>21.0</v>
+      </c>
+      <c r="G10" s="28">
+        <v>26.0</v>
+      </c>
+      <c r="H10" s="28">
+        <v>26.0</v>
+      </c>
+      <c r="I10" s="28">
+        <v>32.0</v>
+      </c>
+      <c r="J10" s="28">
+        <v>36.0</v>
+      </c>
+      <c r="K10" s="28">
+        <v>37.0</v>
+      </c>
+      <c r="L10" s="28">
+        <v>45.0</v>
+      </c>
+      <c r="M10" s="28">
+        <v>37.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="28">
+        <v>142.0</v>
+      </c>
+      <c r="D11" s="28">
+        <v>159.0</v>
+      </c>
+      <c r="E11" s="28">
+        <v>165.0</v>
+      </c>
+      <c r="F11" s="28">
+        <v>95.0</v>
+      </c>
+      <c r="G11" s="28">
+        <v>138.0</v>
+      </c>
+      <c r="H11" s="28">
+        <v>144.0</v>
+      </c>
+      <c r="I11" s="28">
+        <v>24.0</v>
+      </c>
+      <c r="J11" s="28">
+        <v>33.0</v>
+      </c>
+      <c r="K11" s="28">
+        <v>36.0</v>
+      </c>
+      <c r="L11" s="28">
+        <v>253.0</v>
+      </c>
+      <c r="M11" s="28">
+        <v>37.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="28">
+        <v>44.0</v>
+      </c>
+      <c r="D12" s="28">
+        <v>67.0</v>
+      </c>
+      <c r="E12" s="28">
+        <v>44.0</v>
+      </c>
+      <c r="F12" s="28">
+        <v>59.0</v>
+      </c>
+      <c r="G12" s="28">
+        <v>51.0</v>
+      </c>
+      <c r="H12" s="28">
+        <v>46.0</v>
+      </c>
+      <c r="I12" s="28">
+        <v>54.0</v>
+      </c>
+      <c r="J12" s="28">
+        <v>68.0</v>
+      </c>
+      <c r="K12" s="28">
+        <v>70.0</v>
+      </c>
+      <c r="L12" s="28">
+        <v>72.0</v>
+      </c>
+      <c r="M12" s="28">
+        <v>67.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="74" t="s">
+        <v>232</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="78"/>
+      <c r="C15" s="79">
+        <f t="shared" ref="C15:M15" si="1">C21/C27</f>
+        <v>0.0001339393939</v>
+      </c>
+      <c r="D15" s="79">
+        <f t="shared" si="1"/>
+        <v>0.0008605263158</v>
+      </c>
+      <c r="E15" s="79">
+        <f t="shared" si="1"/>
+        <v>0.0007706185567</v>
+      </c>
+      <c r="F15" s="79">
+        <f t="shared" si="1"/>
+        <v>0.0001256017505</v>
+      </c>
+      <c r="G15" s="79">
+        <f t="shared" si="1"/>
+        <v>0.00006650124069</v>
+      </c>
+      <c r="H15" s="79">
+        <f t="shared" si="1"/>
+        <v>0.000112654321</v>
+      </c>
+      <c r="I15" s="79" t="str">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" s="79">
+        <f t="shared" si="1"/>
+        <v>0.0001032727273</v>
+      </c>
+      <c r="K15" s="80">
+        <f t="shared" si="1"/>
+        <v>0.00009226519337</v>
+      </c>
+      <c r="L15" s="81" t="str">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M15" s="79">
+        <f t="shared" si="1"/>
+        <v>0.02320574163</v>
+      </c>
+      <c r="N15" s="78"/>
+      <c r="O15" s="78"/>
+      <c r="P15" s="78"/>
+      <c r="Q15" s="78"/>
+      <c r="R15" s="78"/>
+      <c r="S15" s="78"/>
+      <c r="T15" s="78"/>
+      <c r="U15" s="78"/>
+      <c r="V15" s="78"/>
+      <c r="W15" s="78"/>
+      <c r="X15" s="78"/>
+      <c r="Y15" s="78"/>
+      <c r="Z15" s="78"/>
+      <c r="AA15" s="78"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="30">
+        <f t="shared" ref="C16:K16" si="2">C22/C28</f>
+        <v>0.06860465116</v>
+      </c>
+      <c r="D16" s="30">
+        <f t="shared" si="2"/>
+        <v>0.1405821918</v>
+      </c>
+      <c r="E16" s="30">
+        <f t="shared" si="2"/>
+        <v>0.0578125</v>
+      </c>
+      <c r="F16" s="30">
+        <f t="shared" si="2"/>
+        <v>0.06094420601</v>
+      </c>
+      <c r="G16" s="30">
+        <f t="shared" si="2"/>
+        <v>0.03015151515</v>
+      </c>
+      <c r="H16" s="30">
+        <f t="shared" si="2"/>
+        <v>0.1113043478</v>
+      </c>
+      <c r="I16" s="30">
+        <f t="shared" si="2"/>
+        <v>0.1905972046</v>
+      </c>
+      <c r="J16" s="30">
+        <f t="shared" si="2"/>
+        <v>0.070703125</v>
+      </c>
+      <c r="K16" s="30">
+        <f t="shared" si="2"/>
+        <v>0.07044025157</v>
+      </c>
+      <c r="L16" s="34">
+        <v>0.112</v>
+      </c>
+      <c r="M16" s="34">
+        <v>0.1404</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="34">
+        <v>0.092</v>
+      </c>
+      <c r="D17" s="34">
+        <v>0.1034</v>
+      </c>
+      <c r="E17" s="34">
+        <v>0.0379</v>
+      </c>
+      <c r="F17" s="34">
+        <v>0.0529</v>
+      </c>
+      <c r="G17" s="34">
+        <v>0.0453</v>
+      </c>
+      <c r="H17" s="34">
+        <v>0.0294</v>
+      </c>
+      <c r="I17" s="34">
+        <v>0.079</v>
+      </c>
+      <c r="J17" s="34">
+        <v>0.0633</v>
+      </c>
+      <c r="K17" s="34">
+        <v>0.054</v>
+      </c>
+      <c r="L17" s="34">
+        <v>0.1306</v>
+      </c>
+      <c r="M17" s="34">
+        <v>0.1133</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="34">
+        <v>0.0911</v>
+      </c>
+      <c r="D18" s="34">
+        <v>0.0857</v>
+      </c>
+      <c r="E18" s="34">
+        <v>0.0945</v>
+      </c>
+      <c r="F18" s="34">
+        <v>0.0823</v>
+      </c>
+      <c r="G18" s="34">
+        <v>0.1458</v>
+      </c>
+      <c r="H18" s="34">
+        <v>0.0764</v>
+      </c>
+      <c r="I18" s="34">
+        <v>0.0587</v>
+      </c>
+      <c r="J18" s="34">
+        <v>0.066</v>
+      </c>
+      <c r="K18" s="34">
+        <v>0.0716</v>
+      </c>
+      <c r="L18" s="34">
+        <v>0.0703</v>
+      </c>
+      <c r="M18" s="34">
+        <v>0.0663</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="82" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="C21" s="28">
+        <v>442.0</v>
+      </c>
+      <c r="D21" s="28">
+        <v>3270.0</v>
+      </c>
+      <c r="E21" s="28">
+        <v>2990.0</v>
+      </c>
+      <c r="F21" s="28">
+        <v>574.0</v>
+      </c>
+      <c r="G21" s="28">
+        <v>268.0</v>
+      </c>
+      <c r="H21" s="28">
+        <v>365.0</v>
+      </c>
+      <c r="I21" s="28">
+        <v>236.0</v>
+      </c>
+      <c r="J21" s="28">
+        <v>284.0</v>
+      </c>
+      <c r="K21" s="28">
+        <v>167.0</v>
+      </c>
+      <c r="L21" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="M21" s="80">
+        <f>69+28</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="28">
+        <v>118000.0</v>
+      </c>
+      <c r="D22" s="28">
+        <v>821000.0</v>
+      </c>
+      <c r="E22" s="28">
+        <v>111000.0</v>
+      </c>
+      <c r="F22" s="28">
+        <v>142000.0</v>
+      </c>
+      <c r="G22" s="28">
+        <v>39800.0</v>
+      </c>
+      <c r="H22" s="28">
+        <v>384000.0</v>
+      </c>
+      <c r="I22" s="28">
+        <v>1500000.0</v>
+      </c>
+      <c r="J22" s="28">
+        <v>181000.0</v>
+      </c>
+      <c r="K22" s="28">
+        <v>112000.0</v>
+      </c>
+      <c r="L22" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="M22" s="80">
+        <f>168315+2444+28577</f>
+        <v>199336</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="28">
+        <v>99900.0</v>
+      </c>
+      <c r="D23" s="28">
+        <v>232000.0</v>
+      </c>
+      <c r="E23" s="28">
+        <v>148000.0</v>
+      </c>
+      <c r="F23" s="28">
+        <v>225000.0</v>
+      </c>
+      <c r="G23" s="28">
+        <v>223000.0</v>
+      </c>
+      <c r="H23" s="28">
+        <v>150000.0</v>
+      </c>
+      <c r="I23" s="28">
+        <v>211000.0</v>
+      </c>
+      <c r="J23" s="28">
+        <v>372000.0</v>
+      </c>
+      <c r="K23" s="28">
+        <v>371000.0</v>
+      </c>
+      <c r="L23" s="28">
+        <v>500802.0</v>
+      </c>
+      <c r="M23" s="28">
+        <v>560437.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="28">
+        <v>18000.0</v>
+      </c>
+      <c r="D24" s="28">
+        <v>61900.0</v>
+      </c>
+      <c r="E24" s="28">
+        <v>57300.0</v>
+      </c>
+      <c r="F24" s="28">
+        <v>77600.0</v>
+      </c>
+      <c r="G24" s="28">
+        <v>107000.0</v>
+      </c>
+      <c r="H24" s="28">
+        <v>67400.0</v>
+      </c>
+      <c r="I24" s="28">
+        <v>203000.0</v>
+      </c>
+      <c r="J24" s="28">
+        <v>241000.0</v>
+      </c>
+      <c r="K24" s="28">
+        <v>310000.0</v>
+      </c>
+      <c r="L24" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="M24" s="28">
+        <v>281946.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="82" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="C27" s="28">
+        <v>3300000.0</v>
+      </c>
+      <c r="D27" s="28">
+        <v>3800000.0</v>
+      </c>
+      <c r="E27" s="28">
+        <v>3880000.0</v>
+      </c>
+      <c r="F27" s="28">
+        <v>4570000.0</v>
+      </c>
+      <c r="G27" s="28">
+        <v>4030000.0</v>
+      </c>
+      <c r="H27" s="28">
+        <v>3240000.0</v>
+      </c>
+      <c r="I27" s="29"/>
+      <c r="J27" s="28">
+        <v>2750000.0</v>
+      </c>
+      <c r="K27" s="28">
+        <v>1810000.0</v>
+      </c>
+      <c r="L27" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="M27" s="28">
+        <v>4180.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="28">
+        <v>1720000.0</v>
+      </c>
+      <c r="D28" s="28">
+        <v>5840000.0</v>
+      </c>
+      <c r="E28" s="28">
+        <v>1920000.0</v>
+      </c>
+      <c r="F28" s="28">
+        <v>2330000.0</v>
+      </c>
+      <c r="G28" s="28">
+        <v>1320000.0</v>
+      </c>
+      <c r="H28" s="28">
+        <v>3450000.0</v>
+      </c>
+      <c r="I28" s="28">
+        <v>7870000.0</v>
+      </c>
+      <c r="J28" s="28">
+        <v>2560000.0</v>
+      </c>
+      <c r="K28" s="28">
+        <v>1590000.0</v>
+      </c>
+      <c r="L28" s="28">
+        <v>1882420.0</v>
+      </c>
+      <c r="M28" s="29"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="D29" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="E29" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="F29" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="G29" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="H29" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="I29" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="J29" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="K29" s="28">
+        <v>5940000.0</v>
+      </c>
+      <c r="L29" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="M29" s="75" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="D30" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="E30" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="F30" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="G30" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="H30" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="I30" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="J30" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="K30" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="L30" s="28">
+        <v>356521.0</v>
+      </c>
+      <c r="M30" s="75" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="28"/>
+      <c r="M31" s="29"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>